<commit_message>
Update 3Di database schema 219 to schema 300.xlsx
</commit_message>
<xml_diff>
--- a/source/other/3Di database schema 219 to schema 300.xlsx
+++ b/source/other/3Di database schema 219 to schema 300.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nelenschuurmans.sharepoint.com/sites/IT/Shared Documents/3Di/3di_ontwikkelingen/Database schema 300/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leendert.vanwolfswin\Documents\GitHub\threedi-docs\source\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1928" documentId="8_{61EAA967-5DD5-41C3-ABF7-603BD99DD164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{511AA483-62C8-4895-9058-2863724E7A2A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06466D5C-604C-430C-8D1E-1B739A913A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="396" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="396" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schema 219" sheetId="45" r:id="rId1"/>
@@ -437,6 +437,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Contains CSV-style data for tabulated / YZ cross-sections; </t>
@@ -447,6 +448,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>height, width</t>
@@ -456,6 +458,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> pairs for tabulated; </t>
@@ -466,6 +469,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>y, z</t>
@@ -475,6 +479,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> pairs for YZ</t>
@@ -1644,9 +1649,6 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
-  </si>
-  <si>
-    <t>Possible values: "s1", "vol1"</t>
   </si>
   <si>
     <t>measure_map</t>
@@ -1992,12 +1994,15 @@
   <si>
     <t>migrated to column (schema 300)</t>
   </si>
+  <si>
+    <t>Possible values: "water_level", "volume"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -2040,19 +2045,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2153,8 +2145,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2689,16 +2681,16 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3631,10 +3623,10 @@
         <v>422</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -3642,10 +3634,10 @@
         <v>423</v>
       </c>
       <c r="B56" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D56" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E56" t="s">
         <v>6</v>
@@ -3662,7 +3654,7 @@
         <v>424</v>
       </c>
       <c r="B57" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D57" t="s">
         <v>5</v>
@@ -3682,10 +3674,10 @@
         <v>425</v>
       </c>
       <c r="B58" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D58" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E58" t="s">
         <v>116</v>
@@ -3702,7 +3694,7 @@
         <v>426</v>
       </c>
       <c r="B59" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D59" t="s">
         <v>308</v>
@@ -3722,10 +3714,10 @@
         <v>427</v>
       </c>
       <c r="B60" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D60" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E60" t="s">
         <v>117</v>
@@ -3742,10 +3734,10 @@
         <v>428</v>
       </c>
       <c r="B61" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D61" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E61" t="s">
         <v>116</v>
@@ -3762,10 +3754,10 @@
         <v>429</v>
       </c>
       <c r="B62" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D62" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E62" t="s">
         <v>116</v>
@@ -3782,10 +3774,10 @@
         <v>430</v>
       </c>
       <c r="B63" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D63" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E63" t="s">
         <v>117</v>
@@ -3802,10 +3794,10 @@
         <v>431</v>
       </c>
       <c r="B64" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D64" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E64" t="s">
         <v>117</v>
@@ -3822,7 +3814,7 @@
         <v>432</v>
       </c>
       <c r="B65" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="66" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3830,10 +3822,10 @@
         <v>433</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -3841,10 +3833,10 @@
         <v>434</v>
       </c>
       <c r="B67" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D67" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E67" t="s">
         <v>6</v>
@@ -3861,7 +3853,7 @@
         <v>435</v>
       </c>
       <c r="B68" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D68" t="s">
         <v>5</v>
@@ -3881,7 +3873,7 @@
         <v>436</v>
       </c>
       <c r="B69" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D69" t="s">
         <v>414</v>
@@ -3901,11 +3893,11 @@
         <v>437</v>
       </c>
       <c r="B70" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C70"/>
       <c r="D70" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E70" t="s">
         <v>120</v>
@@ -3922,10 +3914,10 @@
         <v>438</v>
       </c>
       <c r="B71" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D71" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E71" t="s">
         <v>120</v>
@@ -3942,10 +3934,10 @@
         <v>439</v>
       </c>
       <c r="B72" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D72" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E72" t="s">
         <v>117</v>
@@ -3962,10 +3954,10 @@
         <v>440</v>
       </c>
       <c r="B73" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D73" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E73" t="s">
         <v>117</v>
@@ -3982,10 +3974,10 @@
         <v>441</v>
       </c>
       <c r="B74" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D74" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E74" t="s">
         <v>120</v>
@@ -4002,7 +3994,7 @@
         <v>442</v>
       </c>
       <c r="B75" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D75" t="s">
         <v>148</v>
@@ -4022,10 +4014,10 @@
         <v>443</v>
       </c>
       <c r="B76" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D76" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E76" t="s">
         <v>116</v>
@@ -4042,7 +4034,7 @@
         <v>444</v>
       </c>
       <c r="B77" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="78" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4050,10 +4042,10 @@
         <v>445</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -4061,10 +4053,10 @@
         <v>446</v>
       </c>
       <c r="B79" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D79" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E79" t="s">
         <v>6</v>
@@ -4081,7 +4073,7 @@
         <v>447</v>
       </c>
       <c r="B80" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D80" t="s">
         <v>5</v>
@@ -4101,7 +4093,7 @@
         <v>448</v>
       </c>
       <c r="B81" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D81" t="s">
         <v>1</v>
@@ -4121,7 +4113,7 @@
         <v>449</v>
       </c>
       <c r="B82" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D82" t="s">
         <v>136</v>
@@ -4141,7 +4133,7 @@
         <v>450</v>
       </c>
       <c r="B83" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4149,10 +4141,10 @@
         <v>451</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -4160,10 +4152,10 @@
         <v>452</v>
       </c>
       <c r="B85" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D85" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E85" t="s">
         <v>6</v>
@@ -4180,7 +4172,7 @@
         <v>453</v>
       </c>
       <c r="B86" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D86" t="s">
         <v>5</v>
@@ -4200,7 +4192,7 @@
         <v>454</v>
       </c>
       <c r="B87" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="88" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4243,7 +4235,7 @@
         <v>411</v>
       </c>
       <c r="D90" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E90" t="s">
         <v>6</v>
@@ -4263,7 +4255,7 @@
         <v>411</v>
       </c>
       <c r="D91" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E91" t="s">
         <v>162</v>
@@ -4303,16 +4295,16 @@
         <v>411</v>
       </c>
       <c r="D93" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E93" t="s">
         <v>14</v>
       </c>
       <c r="F93" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -4328,10 +4320,10 @@
         <v>462</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -4339,7 +4331,7 @@
         <v>463</v>
       </c>
       <c r="B96" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D96" t="s">
         <v>5</v>
@@ -4359,13 +4351,13 @@
         <v>464</v>
       </c>
       <c r="B97" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D97" t="s">
         <v>414</v>
       </c>
       <c r="E97" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F97" t="s">
         <v>410</v>
@@ -4379,10 +4371,10 @@
         <v>465</v>
       </c>
       <c r="B98" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D98" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E98" t="s">
         <v>14</v>
@@ -4391,7 +4383,7 @@
         <v>149</v>
       </c>
       <c r="G98" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -4399,10 +4391,10 @@
         <v>466</v>
       </c>
       <c r="B99" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D99" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E99" t="s">
         <v>14</v>
@@ -4411,7 +4403,7 @@
         <v>149</v>
       </c>
       <c r="G99" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -4419,19 +4411,19 @@
         <v>467</v>
       </c>
       <c r="B100" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D100" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E100" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F100" t="s">
         <v>149</v>
       </c>
       <c r="G100" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -4439,19 +4431,19 @@
         <v>468</v>
       </c>
       <c r="B101" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D101" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E101" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F101" t="s">
         <v>149</v>
       </c>
       <c r="G101" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -4459,7 +4451,7 @@
         <v>469</v>
       </c>
       <c r="B102" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D102" t="s">
         <v>148</v>
@@ -4479,10 +4471,10 @@
         <v>470</v>
       </c>
       <c r="B103" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D103" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E103" t="s">
         <v>6</v>
@@ -4491,7 +4483,7 @@
         <v>149</v>
       </c>
       <c r="G103" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -4499,10 +4491,10 @@
         <v>471</v>
       </c>
       <c r="B104" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D104" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E104" t="s">
         <v>85</v>
@@ -4511,7 +4503,7 @@
         <v>149</v>
       </c>
       <c r="G104" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="105" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4519,11 +4511,11 @@
         <v>472</v>
       </c>
       <c r="B105" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C105"/>
       <c r="D105" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E105" t="s">
         <v>85</v>
@@ -4532,7 +4524,7 @@
         <v>149</v>
       </c>
       <c r="G105" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
@@ -4540,7 +4532,7 @@
         <v>473</v>
       </c>
       <c r="B106" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="107" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4548,10 +4540,10 @@
         <v>474</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
@@ -4559,7 +4551,7 @@
         <v>475</v>
       </c>
       <c r="B108" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D108" t="s">
         <v>5</v>
@@ -4579,13 +4571,13 @@
         <v>476</v>
       </c>
       <c r="B109" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D109" t="s">
         <v>414</v>
       </c>
       <c r="E109" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F109" t="s">
         <v>17</v>
@@ -4599,10 +4591,10 @@
         <v>477</v>
       </c>
       <c r="B110" t="s">
+        <v>454</v>
+      </c>
+      <c r="D110" t="s">
         <v>455</v>
-      </c>
-      <c r="D110" t="s">
-        <v>456</v>
       </c>
       <c r="E110" t="s">
         <v>14</v>
@@ -4619,10 +4611,10 @@
         <v>478</v>
       </c>
       <c r="B111" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D111" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E111" t="s">
         <v>14</v>
@@ -4639,10 +4631,10 @@
         <v>479</v>
       </c>
       <c r="B112" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D112" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E112" t="s">
         <v>14</v>
@@ -4659,10 +4651,10 @@
         <v>480</v>
       </c>
       <c r="B113" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D113" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E113" t="s">
         <v>14</v>
@@ -4679,13 +4671,13 @@
         <v>481</v>
       </c>
       <c r="B114" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D114" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E114" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F114" t="s">
         <v>17</v>
@@ -4699,7 +4691,7 @@
         <v>482</v>
       </c>
       <c r="B115" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D115" t="s">
         <v>148</v>
@@ -4719,13 +4711,13 @@
         <v>483</v>
       </c>
       <c r="B116" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D116" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E116" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F116" t="s">
         <v>17</v>
@@ -4739,13 +4731,13 @@
         <v>484</v>
       </c>
       <c r="B117" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D117" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E117" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F117" t="s">
         <v>17</v>
@@ -4759,7 +4751,7 @@
         <v>485</v>
       </c>
       <c r="B118" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="119" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4767,10 +4759,10 @@
         <v>486</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
@@ -4778,7 +4770,7 @@
         <v>487</v>
       </c>
       <c r="B120" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D120" t="s">
         <v>5</v>
@@ -4798,10 +4790,10 @@
         <v>488</v>
       </c>
       <c r="B121" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D121" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E121" t="s">
         <v>117</v>
@@ -4810,7 +4802,7 @@
         <v>147</v>
       </c>
       <c r="G121" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
@@ -4818,19 +4810,19 @@
         <v>489</v>
       </c>
       <c r="B122" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D122" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E122" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F122" t="s">
         <v>147</v>
       </c>
       <c r="G122" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
@@ -4838,13 +4830,13 @@
         <v>490</v>
       </c>
       <c r="B123" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D123" t="s">
         <v>414</v>
       </c>
       <c r="E123" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F123" t="s">
         <v>410</v>
@@ -4858,19 +4850,19 @@
         <v>491</v>
       </c>
       <c r="B124" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D124" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E124" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F124" t="s">
         <v>147</v>
       </c>
       <c r="G124" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
@@ -4878,7 +4870,7 @@
         <v>492</v>
       </c>
       <c r="B125" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D125" t="s">
         <v>148</v>
@@ -4898,10 +4890,10 @@
         <v>493</v>
       </c>
       <c r="B126" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D126" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E126" t="s">
         <v>6</v>
@@ -4910,7 +4902,7 @@
         <v>147</v>
       </c>
       <c r="G126" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="127" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4918,7 +4910,7 @@
         <v>494</v>
       </c>
       <c r="B127" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C127"/>
       <c r="D127"/>
@@ -4931,10 +4923,10 @@
         <v>495</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -4942,7 +4934,7 @@
         <v>496</v>
       </c>
       <c r="B129" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D129" t="s">
         <v>5</v>
@@ -4962,13 +4954,13 @@
         <v>497</v>
       </c>
       <c r="B130" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D130" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E130" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F130" t="s">
         <v>17</v>
@@ -4982,10 +4974,10 @@
         <v>498</v>
       </c>
       <c r="B131" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D131" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E131" t="s">
         <v>117</v>
@@ -5002,7 +4994,7 @@
         <v>499</v>
       </c>
       <c r="B132" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D132" t="s">
         <v>148</v>
@@ -5022,10 +5014,10 @@
         <v>500</v>
       </c>
       <c r="B133" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D133" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E133" t="s">
         <v>6</v>
@@ -5042,7 +5034,7 @@
         <v>501</v>
       </c>
       <c r="B134" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="135" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11912,10 +11904,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4749160C-9EBF-4F37-98A1-EE8DDCB35C10}">
   <dimension ref="A1:K583"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F9" sqref="F9"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11936,25 +11928,25 @@
         <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>479</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K1" s="10" t="s">
         <v>3</v>
@@ -12027,7 +12019,7 @@
         <v>No</v>
       </c>
       <c r="J4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>405</v>
@@ -12287,7 +12279,7 @@
         <v>New</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -12535,7 +12527,7 @@
         <v>New</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -13019,7 +13011,7 @@
         <v>No</v>
       </c>
       <c r="K48" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -13043,7 +13035,7 @@
         <v>No</v>
       </c>
       <c r="K49" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
@@ -13118,10 +13110,10 @@
         <v>Yes</v>
       </c>
       <c r="J52" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K52" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
@@ -13609,13 +13601,13 @@
         <v>Yes</v>
       </c>
       <c r="I73" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J73" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K73" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -13642,13 +13634,13 @@
         <v>Yes</v>
       </c>
       <c r="I74" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J74" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K74" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -13675,7 +13667,7 @@
         <v>Yes</v>
       </c>
       <c r="J75" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K75" s="12" t="s">
         <v>130</v>
@@ -13705,10 +13697,10 @@
         <v>Yes</v>
       </c>
       <c r="J76" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K76" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -13735,7 +13727,7 @@
         <v>Yes</v>
       </c>
       <c r="J77" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K77" s="9" t="s">
         <v>134</v>
@@ -14329,10 +14321,10 @@
         <v>Yes</v>
       </c>
       <c r="J102" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K102" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="103" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -14363,10 +14355,10 @@
         <v>Yes</v>
       </c>
       <c r="J103" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K103" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="104" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -14393,7 +14385,7 @@
         <v>Yes</v>
       </c>
       <c r="J104" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K104" s="9" t="s">
         <v>135</v>
@@ -14942,7 +14934,7 @@
         <v>Yes</v>
       </c>
       <c r="K129" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.3">
@@ -15814,7 +15806,7 @@
         <v>No</v>
       </c>
       <c r="J169" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K169" s="9" t="s">
         <v>406</v>
@@ -15895,7 +15887,7 @@
         <v>Yes</v>
       </c>
       <c r="J172" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K172" s="9" t="s">
         <v>406</v>
@@ -15976,7 +15968,7 @@
         <v>No</v>
       </c>
       <c r="J175" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K175" s="9" t="s">
         <v>406</v>
@@ -16058,7 +16050,7 @@
       </c>
       <c r="I178"/>
       <c r="J178" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K178" s="9" t="s">
         <v>406</v>
@@ -16139,7 +16131,7 @@
         <v>No</v>
       </c>
       <c r="J181" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K181" s="9" t="s">
         <v>406</v>
@@ -16220,7 +16212,7 @@
         <v>No</v>
       </c>
       <c r="J184" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K184" s="9" t="s">
         <v>406</v>
@@ -16276,7 +16268,7 @@
         <v>No</v>
       </c>
       <c r="J186" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K186" s="9" t="s">
         <v>406</v>
@@ -16434,7 +16426,7 @@
         <v>No</v>
       </c>
       <c r="J193" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K193" s="9" t="s">
         <v>406</v>
@@ -16515,7 +16507,7 @@
         <v>Yes</v>
       </c>
       <c r="J196" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K196" s="9" t="s">
         <v>406</v>
@@ -16623,7 +16615,7 @@
         <v>No</v>
       </c>
       <c r="J201" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K201" s="9" t="s">
         <v>406</v>
@@ -16731,7 +16723,7 @@
         <v>No</v>
       </c>
       <c r="J206" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K206" s="9" t="s">
         <v>406</v>
@@ -16837,7 +16829,7 @@
         <v>No</v>
       </c>
       <c r="J210" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K210" s="9" t="s">
         <v>406</v>
@@ -17039,7 +17031,7 @@
         <v>New</v>
       </c>
       <c r="K219" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="220" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -17347,7 +17339,7 @@
         <v>New</v>
       </c>
       <c r="K232" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="233" spans="1:11" x14ac:dyDescent="0.3">
@@ -17774,7 +17766,7 @@
         <v>No</v>
       </c>
       <c r="K251" s="9" t="s">
-        <v>416</v>
+        <v>493</v>
       </c>
     </row>
     <row r="252" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -17817,10 +17809,10 @@
         <v>527</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C254" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D254" s="5"/>
       <c r="E254" s="5"/>
@@ -17835,7 +17827,7 @@
         <v>528</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C255" s="2"/>
       <c r="D255" s="2" t="s">
@@ -17860,7 +17852,7 @@
         <v>529</v>
       </c>
       <c r="B256" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D256" t="s">
         <v>24</v>
@@ -17879,7 +17871,7 @@
         <v>New</v>
       </c>
       <c r="K256" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="257" spans="1:11" x14ac:dyDescent="0.3">
@@ -17887,7 +17879,7 @@
         <v>530</v>
       </c>
       <c r="B257" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D257" t="s">
         <v>10</v>
@@ -17911,7 +17903,7 @@
         <v>531</v>
       </c>
       <c r="B258" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D258" t="s">
         <v>8</v>
@@ -17935,10 +17927,10 @@
         <v>532</v>
       </c>
       <c r="B259" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D259" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E259" t="s">
         <v>120</v>
@@ -17947,7 +17939,7 @@
         <v>411</v>
       </c>
       <c r="G259" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H259" t="str">
         <f t="shared" si="22"/>
@@ -17959,10 +17951,10 @@
         <v>533</v>
       </c>
       <c r="B260" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D260" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E260" t="s">
         <v>116</v>
@@ -17983,26 +17975,26 @@
         <v>534</v>
       </c>
       <c r="B261" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D261" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E261" t="s">
         <v>117</v>
       </c>
       <c r="F261" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G261" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H261" t="str">
         <f t="shared" si="22"/>
         <v>No</v>
       </c>
       <c r="K261" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="262" spans="1:11" x14ac:dyDescent="0.3">
@@ -18010,19 +18002,19 @@
         <v>535</v>
       </c>
       <c r="B262" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D262" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E262" t="s">
         <v>6</v>
       </c>
       <c r="F262" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G262" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H262" t="str">
         <f t="shared" si="22"/>
@@ -18034,7 +18026,7 @@
         <v>536</v>
       </c>
       <c r="B263" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D263" t="s">
         <v>118</v>
@@ -18096,7 +18088,7 @@
         <v>116</v>
       </c>
       <c r="F266" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G266" t="s">
         <v>5</v>
@@ -18120,7 +18112,7 @@
         <v>33</v>
       </c>
       <c r="F267" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G267" t="s">
         <v>22</v>
@@ -18186,16 +18178,16 @@
         <v>149</v>
       </c>
       <c r="D270" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E270" t="s">
         <v>117</v>
       </c>
       <c r="F270" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G270" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H270" t="str">
         <f t="shared" si="23"/>
@@ -18210,16 +18202,16 @@
         <v>149</v>
       </c>
       <c r="D271" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E271" s="6" t="s">
         <v>120</v>
       </c>
       <c r="F271" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G271" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H271" t="str">
         <f t="shared" si="23"/>
@@ -18230,10 +18222,10 @@
         <v>Yes</v>
       </c>
       <c r="J271" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K271" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="272" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
@@ -18244,16 +18236,16 @@
         <v>149</v>
       </c>
       <c r="D272" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E272" s="6" t="s">
         <v>120</v>
       </c>
       <c r="F272" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G272" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H272" t="str">
         <f t="shared" si="23"/>
@@ -18264,10 +18256,10 @@
         <v>Yes</v>
       </c>
       <c r="J272" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K272" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="273" spans="1:11" x14ac:dyDescent="0.3">
@@ -18278,16 +18270,16 @@
         <v>149</v>
       </c>
       <c r="D273" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E273" t="s">
         <v>85</v>
       </c>
       <c r="F273" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G273" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H273" t="str">
         <f t="shared" si="23"/>
@@ -18302,16 +18294,16 @@
         <v>149</v>
       </c>
       <c r="D274" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E274" t="s">
         <v>85</v>
       </c>
       <c r="F274" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G274" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H274" t="str">
         <f t="shared" si="23"/>
@@ -18326,16 +18318,16 @@
         <v>149</v>
       </c>
       <c r="D275" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E275" t="s">
         <v>120</v>
       </c>
       <c r="F275" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G275" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H275" t="str">
         <f t="shared" si="23"/>
@@ -18350,16 +18342,16 @@
         <v>149</v>
       </c>
       <c r="D276" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E276" t="s">
         <v>120</v>
       </c>
       <c r="F276" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G276" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H276" t="str">
         <f t="shared" si="23"/>
@@ -18380,7 +18372,7 @@
         <v>117</v>
       </c>
       <c r="F277" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G277" t="s">
         <v>148</v>
@@ -18390,10 +18382,10 @@
         <v>No</v>
       </c>
       <c r="J277" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K277" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="278" spans="1:11" x14ac:dyDescent="0.3">
@@ -18404,16 +18396,16 @@
         <v>149</v>
       </c>
       <c r="D278" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E278" t="s">
         <v>116</v>
       </c>
       <c r="F278" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G278" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H278" t="str">
         <f t="shared" si="23"/>
@@ -18560,7 +18552,7 @@
         <v>No</v>
       </c>
       <c r="J285" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K285" s="9" t="s">
         <v>406</v>
@@ -18691,7 +18683,7 @@
         <v>Yes</v>
       </c>
       <c r="J290" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K290" s="9" t="s">
         <v>406</v>
@@ -18870,7 +18862,7 @@
         <v>New</v>
       </c>
       <c r="K297" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="298" spans="1:11" x14ac:dyDescent="0.3">
@@ -19021,7 +19013,7 @@
         <v>Yes</v>
       </c>
       <c r="K303" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="304" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -19049,7 +19041,7 @@
         <v>Yes</v>
       </c>
       <c r="K304" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="305" spans="1:11" x14ac:dyDescent="0.3">
@@ -19102,7 +19094,7 @@
         <v>Yes</v>
       </c>
       <c r="K306" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="307" spans="1:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -19131,7 +19123,7 @@
       </c>
       <c r="I307"/>
       <c r="K307" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="308" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -19159,7 +19151,7 @@
         <v>Yes</v>
       </c>
       <c r="K308" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="309" spans="1:11" x14ac:dyDescent="0.3">
@@ -20443,10 +20435,10 @@
         <v>Yes</v>
       </c>
       <c r="I363" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J363" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K363" s="9" t="s">
         <v>126</v>
@@ -20476,10 +20468,10 @@
         <v>Yes</v>
       </c>
       <c r="I364" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J364" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K364" s="9" t="s">
         <v>126</v>
@@ -20509,7 +20501,7 @@
         <v>Yes</v>
       </c>
       <c r="J365" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K365" s="9" t="s">
         <v>135</v>
@@ -21069,10 +21061,10 @@
         <v>Yes</v>
       </c>
       <c r="I389" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J389" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K389" s="9" t="s">
         <v>126</v>
@@ -21102,10 +21094,10 @@
         <v>Yes</v>
       </c>
       <c r="I390" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J390" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K390" s="9" t="s">
         <v>126</v>
@@ -21135,7 +21127,7 @@
         <v>Yes</v>
       </c>
       <c r="J391" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K391" s="9" t="s">
         <v>135</v>
@@ -21266,7 +21258,7 @@
         <v>New</v>
       </c>
       <c r="K396" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="397" spans="1:11" x14ac:dyDescent="0.3">
@@ -21466,10 +21458,10 @@
         <v>Yes</v>
       </c>
       <c r="J405" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K405" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="406" spans="1:11" x14ac:dyDescent="0.3">
@@ -22468,7 +22460,7 @@
         <v>Yes</v>
       </c>
       <c r="K450" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="451" spans="1:11" x14ac:dyDescent="0.3">
@@ -22644,7 +22636,7 @@
         <v>Yes</v>
       </c>
       <c r="K458" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="459" spans="1:11" x14ac:dyDescent="0.3">
@@ -23094,7 +23086,7 @@
         <v>116</v>
       </c>
       <c r="F479" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G479" t="s">
         <v>5</v>
@@ -23120,10 +23112,10 @@
         <v>33</v>
       </c>
       <c r="F480" t="s">
+        <v>435</v>
+      </c>
+      <c r="G480" t="s">
         <v>436</v>
-      </c>
-      <c r="G480" t="s">
-        <v>437</v>
       </c>
       <c r="H480" t="str">
         <f t="shared" si="27"/>
@@ -23186,16 +23178,16 @@
         <v>147</v>
       </c>
       <c r="D483" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E483" t="s">
         <v>117</v>
       </c>
       <c r="F483" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G483" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H483" t="str">
         <f t="shared" si="27"/>
@@ -23210,26 +23202,26 @@
         <v>147</v>
       </c>
       <c r="D484" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E484" t="s">
         <v>117</v>
       </c>
       <c r="F484" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G484" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H484" t="str">
         <f t="shared" si="27"/>
         <v>No</v>
       </c>
       <c r="J484" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K484" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="485" spans="1:11" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -23247,7 +23239,7 @@
         <v>117</v>
       </c>
       <c r="F485" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G485" t="s">
         <v>148</v>
@@ -23258,10 +23250,10 @@
       </c>
       <c r="I485"/>
       <c r="J485" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K485" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="486" spans="1:11" x14ac:dyDescent="0.3">
@@ -23272,16 +23264,16 @@
         <v>147</v>
       </c>
       <c r="D486" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E486" t="s">
         <v>116</v>
       </c>
       <c r="F486" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G486" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H486" t="str">
         <f t="shared" si="27"/>
@@ -23296,16 +23288,16 @@
         <v>147</v>
       </c>
       <c r="D487" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E487" t="s">
         <v>117</v>
       </c>
       <c r="F487" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G487" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H487" t="str">
         <f t="shared" si="27"/>
@@ -23692,7 +23684,7 @@
         <v>No</v>
       </c>
       <c r="J505" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K505" s="9" t="s">
         <v>406</v>
@@ -23748,7 +23740,7 @@
         <v>No</v>
       </c>
       <c r="J507" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K507" s="9" t="s">
         <v>406</v>
@@ -23804,7 +23796,7 @@
         <v>No</v>
       </c>
       <c r="J509" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K509" s="9" t="s">
         <v>406</v>
@@ -23860,7 +23852,7 @@
         <v>No</v>
       </c>
       <c r="J511" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K511" s="9" t="s">
         <v>406</v>
@@ -24276,10 +24268,10 @@
         <v>Yes</v>
       </c>
       <c r="I529" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J529" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K529" s="9" t="s">
         <v>126</v>
@@ -24309,10 +24301,10 @@
         <v>Yes</v>
       </c>
       <c r="I530" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J530" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K530" s="9" t="s">
         <v>126</v>
@@ -24342,7 +24334,7 @@
         <v>Yes</v>
       </c>
       <c r="J531" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K531" s="9" t="s">
         <v>135</v>
@@ -24399,7 +24391,7 @@
         <v>New</v>
       </c>
       <c r="K533" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="534" spans="1:11" x14ac:dyDescent="0.3">
@@ -24942,12 +24934,12 @@
     <sortCondition ref="B2:B583"/>
     <sortCondition ref="A2:A583"/>
   </sortState>
-  <conditionalFormatting sqref="J4 J52 J73:J77 J102:J104 J169 J172 J175 J196 J201 J206 J210 J271:J272 J277 J285 J290 J363:J365 J389:J391 J405:J406 J484:J485 J505 J529:J531 F1:I1048576">
+  <conditionalFormatting sqref="F1:I1048576 J4 J52 J73:J77 J102:J104 J169 J172 J175 J196 J201 J206 J210 J271:J272 J277 J285 J290 J363:J365 J389:J391 J405:J406 J484:J485 J505 J529:J531">
     <cfRule type="cellIs" dxfId="17" priority="22" operator="equal">
       <formula>"New"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4 J52 J73:J77 J102:J104 J169 J172 J175 J196 J201 J206 J210 J271:J272 J277 J285 J290 J363:J365 J389:J391 J405:J406 J484:J485 J505 J529:J531 H1:I1048576">
+  <conditionalFormatting sqref="H1:I1048576 J4 J52 J73:J77 J102:J104 J169 J172 J175 J196 J201 J206 J210 J271:J272 J277 J285 J290 J363:J365 J389:J391 J405:J406 J484:J485 J505 J529:J531">
     <cfRule type="cellIs" dxfId="16" priority="21" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -25021,46 +25013,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cc3eb999-6c4b-460d-8ce9-8d56410e277c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="df0f4e28-0586-400a-aed3-47c84d14dcbf" xsi:nil="true"/>
-    <SharedWithUsers xmlns="df0f4e28-0586-400a-aed3-47c84d14dcbf">
-      <UserInfo>
-        <DisplayName>Nicolette Volp</DisplayName>
-        <AccountId>32</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jelle Prins</DisplayName>
-        <AccountId>40</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Martijn Siemerink</DisplayName>
-        <AccountId>24</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Margriet Palm</DisplayName>
-        <AccountId>372</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Leendert van Wolfswinkel</DisplayName>
-        <AccountId>43</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Bram de Vries</DisplayName>
-        <AccountId>214</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25313,21 +25271,52 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cc3eb999-6c4b-460d-8ce9-8d56410e277c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="df0f4e28-0586-400a-aed3-47c84d14dcbf" xsi:nil="true"/>
+    <SharedWithUsers xmlns="df0f4e28-0586-400a-aed3-47c84d14dcbf">
+      <UserInfo>
+        <DisplayName>Nicolette Volp</DisplayName>
+        <AccountId>32</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jelle Prins</DisplayName>
+        <AccountId>40</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Martijn Siemerink</DisplayName>
+        <AccountId>24</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Margriet Palm</DisplayName>
+        <AccountId>372</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Leendert van Wolfswinkel</DisplayName>
+        <AccountId>43</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Bram de Vries</DisplayName>
+        <AccountId>214</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C60C38D0-92BE-4ED4-A808-56AF2E73689C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22D1076F-F0B0-49DB-A9F5-1C61AC2D9C1F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cc3eb999-6c4b-460d-8ce9-8d56410e277c"/>
-    <ds:schemaRef ds:uri="df0f4e28-0586-400a-aed3-47c84d14dcbf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25352,9 +25341,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22D1076F-F0B0-49DB-A9F5-1C61AC2D9C1F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C60C38D0-92BE-4ED4-A808-56AF2E73689C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cc3eb999-6c4b-460d-8ce9-8d56410e277c"/>
+    <ds:schemaRef ds:uri="df0f4e28-0586-400a-aed3-47c84d14dcbf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>